<commit_message>
isim tamam, eğitmen tamam değil
</commit_message>
<xml_diff>
--- a/Python/oguz/skylab-certificate-system-main/list.xlsx
+++ b/Python/oguz/skylab-certificate-system-main/list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtur\Desktop\trashcode\Python\oguz\skylab-certificate-system-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691D2AE7-C963-46E8-867E-AB10298453E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB3DA8-FAE0-4A87-AB41-BA4715A2FAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="2010" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1455" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>onur</t>
   </si>
@@ -29,6 +29,21 @@
   </si>
   <si>
     <t>onurturan.t@gmail.com</t>
+  </si>
+  <si>
+    <t>mustafa</t>
+  </si>
+  <si>
+    <t>aksfmasl</t>
+  </si>
+  <si>
+    <t>mr.turran@gmail.com</t>
+  </si>
+  <si>
+    <t>Umut</t>
+  </si>
+  <si>
+    <t>güzel</t>
   </si>
 </sst>
 </file>
@@ -84,11 +99,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Köprü" xfId="2" builtinId="8"/>
@@ -312,31 +329,43 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -504,6 +533,11 @@
       <c r="C36" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DE754260-EE5D-4E95-81CD-E7E03D442005}"/>
+    <hyperlink ref="C1" r:id="rId2" xr:uid="{91FA8E46-BFBE-4F00-9509-5BFF35C24698}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{AC7C7841-4D21-4A78-A615-B866E2252CE0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>